<commit_message>
BOT; UPDATE DATA (#128)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/kansensya_pcr_1.xlsx
+++ b/static/data/kansensya_pcr_1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file.kobe.local\top\02_作業文書\01_組織\平成31年度\01_市長室\03_広報戦略部\01_広報課\04_HP\コロナ\HP作図\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\201058\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="＿" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">kobe!$A$1:$J$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">kobe!$A$1:$J$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">other!$A$1:$H$23</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -195,19 +195,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>※　16件調査中</t>
-    <rPh sb="4" eb="5">
-      <t>ケン</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>チョウサ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>チュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>※ 患者発生総数【速報含む】は、調査中も含みます。</t>
     <rPh sb="16" eb="19">
       <t>チョウサチュウ</t>
@@ -273,6 +260,19 @@
     </rPh>
     <rPh sb="33" eb="35">
       <t>ゴウケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※　39件調査中</t>
+    <rPh sb="4" eb="5">
+      <t>ケン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>チョウサ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>チュウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -784,11 +784,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -877,7 +877,7 @@
         <v>43932</v>
       </c>
       <c r="B4" s="33">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C4" s="35">
         <v>76</v>
@@ -911,17 +911,17 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="17"/>
       <c r="B6" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B8" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
@@ -972,13 +972,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A58" sqref="A58"/>
+      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2366,7 +2366,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A49" s="3">
         <v>43922</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50" s="3">
         <v>43923</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A51" s="3">
         <v>43924</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
         <v>43925</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
         <v>43926</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
         <v>43927</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
         <v>43928</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
         <v>43929</v>
       </c>
@@ -2622,14 +2622,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
         <v>43930</v>
       </c>
-      <c r="B57" s="32">
+      <c r="B57" s="39">
         <v>63</v>
       </c>
-      <c r="C57" s="32">
+      <c r="C57" s="39">
         <v>688</v>
       </c>
       <c r="D57" s="39">
@@ -2654,7 +2654,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="17">
         <v>43931</v>
       </c>
@@ -2665,10 +2665,10 @@
         <v>718</v>
       </c>
       <c r="D58" s="39">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E58" s="38">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F58" s="9">
         <v>43</v>
@@ -2686,34 +2686,66 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="3"/>
-      <c r="F59" s="9"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A60" s="3"/>
-      <c r="B60" s="9" t="s">
+    <row r="59" spans="1:10" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="34">
+        <v>43932</v>
+      </c>
+      <c r="B59" s="39">
+        <v>20</v>
+      </c>
+      <c r="C59" s="39">
+        <v>738</v>
+      </c>
+      <c r="D59" s="39">
+        <v>14</v>
+      </c>
+      <c r="E59" s="38">
+        <v>113</v>
+      </c>
+      <c r="F59" s="9">
+        <v>43</v>
+      </c>
+      <c r="G59" s="9">
+        <v>39</v>
+      </c>
+      <c r="H59" s="9">
+        <v>4</v>
+      </c>
+      <c r="I59" s="9">
+        <v>0</v>
+      </c>
+      <c r="J59" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="34"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A61" s="3"/>
+      <c r="B61" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D60" s="21"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="22"/>
-      <c r="I60" s="19"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B61" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="23"/>
-      <c r="E61" s="24"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="20"/>
       <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
+      <c r="G61" s="19"/>
       <c r="H61" s="22"/>
       <c r="I61" s="19"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B62" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="D62" s="23"/>
       <c r="E62" s="24"/>
       <c r="F62" s="22"/>
@@ -2721,30 +2753,27 @@
       <c r="H62" s="22"/>
       <c r="I62" s="19"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="D63" s="36"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="44"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="44"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="C64" s="7"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="D63" s="23"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="19"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="D64" s="36"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="33"/>
       <c r="H64" s="44"/>
-      <c r="I64" s="44"/>
+      <c r="I64" s="33"/>
       <c r="J64" s="33"/>
-      <c r="K64" s="6"/>
     </row>
     <row r="65" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C65" s="7"/>
-      <c r="D65" s="40"/>
-      <c r="E65" s="41"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="43"/>
       <c r="F65" s="37"/>
       <c r="G65" s="37"/>
       <c r="H65" s="44"/>
@@ -2769,10 +2798,21 @@
       <c r="E67" s="41"/>
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
-      <c r="H67" s="37"/>
-      <c r="I67" s="37"/>
-      <c r="J67" s="37"/>
+      <c r="H67" s="44"/>
+      <c r="I67" s="44"/>
+      <c r="J67" s="33"/>
       <c r="K67" s="6"/>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="C68" s="7"/>
+      <c r="D68" s="40"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2786,13 +2826,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3603,8 +3643,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B35" s="1" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A34" s="34">
+        <v>43932</v>
+      </c>
+      <c r="B34" s="38">
+        <v>0</v>
+      </c>
+      <c r="C34" s="38">
+        <v>8</v>
+      </c>
+      <c r="D34" s="38">
+        <v>6</v>
+      </c>
+      <c r="E34" s="38">
+        <v>5</v>
+      </c>
+      <c r="F34" s="35">
+        <v>1</v>
+      </c>
+      <c r="G34" s="35">
+        <v>0</v>
+      </c>
+      <c r="H34" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B36" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#153)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/kansensya_pcr_1.xlsx
+++ b/static/data/kansensya_pcr_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="6" r:id="rId1"/>
@@ -18,15 +18,15 @@
     <sheet name="＿" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">kobe!$A$1:$J$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">kobe!$A$1:$J$63</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">other!$A$1:$H$23</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>検査実施人数（累計）　　</t>
     <phoneticPr fontId="1"/>
@@ -36,10 +36,6 @@
     <rPh sb="5" eb="7">
       <t>ルイケイ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>入院中</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -264,7 +260,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>※　39件調査中</t>
+    <t>※　38件調査中</t>
     <rPh sb="4" eb="5">
       <t>ケン</t>
     </rPh>
@@ -273,6 +269,23 @@
     </rPh>
     <rPh sb="7" eb="8">
       <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>入院・入居中</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウイン</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ニュウキョチュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>入院・入居中</t>
+    <rPh sb="3" eb="5">
+      <t>ニュウキョ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -342,7 +355,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -373,9 +386,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -400,35 +410,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -439,9 +425,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -451,32 +434,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,183 +768,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C16:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="20.125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="20.125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" x14ac:dyDescent="0.15">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="16">
+        <v>43930</v>
+      </c>
+      <c r="B2" s="13">
+        <v>90</v>
+      </c>
+      <c r="C2" s="17">
+        <v>84</v>
+      </c>
+      <c r="D2" s="17">
+        <v>56</v>
+      </c>
+      <c r="E2" s="17">
+        <v>51</v>
+      </c>
+      <c r="F2" s="17">
+        <v>5</v>
+      </c>
+      <c r="G2" s="17">
+        <v>0</v>
+      </c>
+      <c r="H2" s="17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="24">
+        <v>43931</v>
+      </c>
+      <c r="B3" s="10">
+        <v>90</v>
+      </c>
+      <c r="C3" s="25">
+        <v>85</v>
+      </c>
+      <c r="D3" s="25">
+        <v>58</v>
+      </c>
+      <c r="E3" s="25">
+        <v>53</v>
+      </c>
+      <c r="F3" s="25">
+        <v>5</v>
+      </c>
+      <c r="G3" s="25">
+        <v>0</v>
+      </c>
+      <c r="H3" s="25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="24">
+        <v>43932</v>
+      </c>
+      <c r="B4" s="23">
+        <v>113</v>
+      </c>
+      <c r="C4" s="9">
+        <v>86</v>
+      </c>
+      <c r="D4" s="19">
+        <v>58</v>
+      </c>
+      <c r="E4" s="19">
+        <v>54</v>
+      </c>
+      <c r="F4" s="19">
+        <v>4</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0</v>
+      </c>
+      <c r="H4" s="19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="24">
+        <v>43933</v>
+      </c>
+      <c r="B5" s="23">
+        <v>121</v>
+      </c>
+      <c r="C5" s="9">
+        <v>86</v>
+      </c>
+      <c r="D5" s="19">
+        <v>58</v>
+      </c>
+      <c r="E5" s="19">
+        <v>54</v>
+      </c>
+      <c r="F5" s="19">
+        <v>4</v>
+      </c>
+      <c r="G5" s="19">
+        <v>9</v>
+      </c>
+      <c r="H5" s="19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="24"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="16"/>
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="17">
-        <v>43930</v>
-      </c>
-      <c r="B2" s="14">
-        <v>90</v>
-      </c>
-      <c r="C2" s="18">
-        <v>76</v>
-      </c>
-      <c r="D2" s="18">
-        <v>49</v>
-      </c>
-      <c r="E2" s="18">
-        <v>44</v>
-      </c>
-      <c r="F2" s="18">
-        <v>5</v>
-      </c>
-      <c r="G2" s="18">
-        <v>0</v>
-      </c>
-      <c r="H2" s="18">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="34">
-        <v>43931</v>
-      </c>
-      <c r="B3" s="11">
-        <v>90</v>
-      </c>
-      <c r="C3" s="35">
-        <v>76</v>
-      </c>
-      <c r="D3" s="35">
-        <v>49</v>
-      </c>
-      <c r="E3" s="35">
-        <v>44</v>
-      </c>
-      <c r="F3" s="35">
-        <v>5</v>
-      </c>
-      <c r="G3" s="35">
-        <v>0</v>
-      </c>
-      <c r="H3" s="35">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="34">
-        <v>43932</v>
-      </c>
-      <c r="B4" s="33">
-        <v>113</v>
-      </c>
-      <c r="C4" s="35">
-        <v>76</v>
-      </c>
-      <c r="D4" s="35">
-        <v>49</v>
-      </c>
-      <c r="E4" s="35">
-        <v>44</v>
-      </c>
-      <c r="F4" s="35">
-        <v>5</v>
-      </c>
-      <c r="G4" s="35">
-        <v>0</v>
-      </c>
-      <c r="H4" s="35">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="34"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="17"/>
-      <c r="B6" s="11" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B7" s="11" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B8" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B11" s="14"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B12" s="14"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B13" s="14"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -972,13 +948,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -990,31 +966,31 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
@@ -2129,10 +2105,10 @@
       <c r="F41" s="4">
         <v>15</v>
       </c>
-      <c r="G41" s="15">
+      <c r="G41" s="14">
         <v>13</v>
       </c>
-      <c r="H41" s="15">
+      <c r="H41" s="14">
         <v>2</v>
       </c>
       <c r="I41" s="4">
@@ -2161,10 +2137,10 @@
       <c r="F42" s="4">
         <v>12</v>
       </c>
-      <c r="G42" s="15">
+      <c r="G42" s="14">
         <v>10</v>
       </c>
-      <c r="H42" s="15">
+      <c r="H42" s="14">
         <v>2</v>
       </c>
       <c r="I42" s="4">
@@ -2193,10 +2169,10 @@
       <c r="F43" s="4">
         <v>9</v>
       </c>
-      <c r="G43" s="15">
+      <c r="G43" s="14">
         <v>7</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H43" s="14">
         <v>2</v>
       </c>
       <c r="I43" s="4">
@@ -2225,10 +2201,10 @@
       <c r="F44" s="4">
         <v>11</v>
       </c>
-      <c r="G44" s="15">
+      <c r="G44" s="14">
         <v>10</v>
       </c>
-      <c r="H44" s="15">
+      <c r="H44" s="14">
         <v>1</v>
       </c>
       <c r="I44" s="4">
@@ -2257,10 +2233,10 @@
       <c r="F45" s="8">
         <v>11</v>
       </c>
-      <c r="G45" s="15">
+      <c r="G45" s="14">
         <v>10</v>
       </c>
-      <c r="H45" s="15">
+      <c r="H45" s="14">
         <v>1</v>
       </c>
       <c r="I45" s="4">
@@ -2289,10 +2265,10 @@
       <c r="F46" s="6">
         <v>13</v>
       </c>
-      <c r="G46" s="15">
+      <c r="G46" s="14">
         <v>12</v>
       </c>
-      <c r="H46" s="15">
+      <c r="H46" s="14">
         <v>1</v>
       </c>
       <c r="I46" s="6">
@@ -2321,10 +2297,10 @@
       <c r="F47" s="6">
         <v>13</v>
       </c>
-      <c r="G47" s="15">
+      <c r="G47" s="14">
         <v>12</v>
       </c>
-      <c r="H47" s="15">
+      <c r="H47" s="14">
         <v>1</v>
       </c>
       <c r="I47" s="6">
@@ -2353,10 +2329,10 @@
       <c r="F48" s="6">
         <v>13</v>
       </c>
-      <c r="G48" s="15">
+      <c r="G48" s="14">
         <v>11</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H48" s="14">
         <v>2</v>
       </c>
       <c r="I48" s="6">
@@ -2366,7 +2342,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" s="3">
         <v>43922</v>
       </c>
@@ -2385,10 +2361,10 @@
       <c r="F49" s="6">
         <v>13</v>
       </c>
-      <c r="G49" s="15">
+      <c r="G49" s="14">
         <v>11</v>
       </c>
-      <c r="H49" s="15">
+      <c r="H49" s="14">
         <v>2</v>
       </c>
       <c r="I49" s="6">
@@ -2398,7 +2374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50" s="3">
         <v>43923</v>
       </c>
@@ -2417,10 +2393,10 @@
       <c r="F50" s="6">
         <v>14</v>
       </c>
-      <c r="G50" s="15">
+      <c r="G50" s="14">
         <v>12</v>
       </c>
-      <c r="H50" s="15">
+      <c r="H50" s="14">
         <v>2</v>
       </c>
       <c r="I50" s="6">
@@ -2430,7 +2406,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51" s="3">
         <v>43924</v>
       </c>
@@ -2449,36 +2425,36 @@
       <c r="F51" s="6">
         <v>17</v>
       </c>
-      <c r="G51" s="15">
+      <c r="G51" s="14">
         <v>15</v>
       </c>
-      <c r="H51" s="15">
+      <c r="H51" s="14">
         <v>2</v>
       </c>
       <c r="I51" s="6">
         <v>0</v>
       </c>
-      <c r="J51" s="29">
+      <c r="J51" s="20">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
         <v>43925</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="13">
         <v>24</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="13">
         <v>507</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="13">
         <v>5</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="25">
         <v>44</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F52" s="25">
         <v>19</v>
       </c>
       <c r="G52" s="9">
@@ -2487,30 +2463,32 @@
       <c r="H52" s="9">
         <v>2</v>
       </c>
-      <c r="I52" s="6">
-        <v>0</v>
-      </c>
-      <c r="J52" s="28">
+      <c r="I52" s="25">
+        <v>0</v>
+      </c>
+      <c r="J52" s="23">
         <v>22</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K52" s="23"/>
+      <c r="L52" s="23"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
         <v>43926</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="13">
         <v>10</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="13">
         <v>517</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="13">
         <v>7</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="25">
         <v>51</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F53" s="25">
         <v>24</v>
       </c>
       <c r="G53" s="9">
@@ -2519,300 +2497,369 @@
       <c r="H53" s="9">
         <v>3</v>
       </c>
-      <c r="I53" s="6">
-        <v>0</v>
-      </c>
-      <c r="J53" s="28">
+      <c r="I53" s="25">
+        <v>0</v>
+      </c>
+      <c r="J53" s="23">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K53" s="23"/>
+      <c r="L53" s="23"/>
+    </row>
+    <row r="54" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
         <v>43927</v>
       </c>
-      <c r="B54" s="32">
+      <c r="B54" s="30">
         <v>25</v>
       </c>
-      <c r="C54" s="32">
+      <c r="C54" s="30">
         <v>542</v>
       </c>
-      <c r="D54" s="36">
+      <c r="D54" s="30">
         <v>5</v>
       </c>
-      <c r="E54" s="35">
+      <c r="E54" s="27">
         <v>56</v>
       </c>
-      <c r="F54" s="44">
+      <c r="F54" s="29">
         <v>33</v>
       </c>
-      <c r="G54" s="33">
+      <c r="G54" s="29">
         <v>29</v>
       </c>
-      <c r="H54" s="44">
+      <c r="H54" s="29">
         <v>4</v>
       </c>
-      <c r="I54" s="33">
-        <v>0</v>
-      </c>
-      <c r="J54" s="33">
+      <c r="I54" s="29">
+        <v>0</v>
+      </c>
+      <c r="J54" s="29">
         <v>22</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K54" s="23"/>
+      <c r="L54" s="23"/>
+    </row>
+    <row r="55" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
         <v>43928</v>
       </c>
-      <c r="B55" s="32">
+      <c r="B55" s="30">
         <v>40</v>
       </c>
-      <c r="C55" s="32">
+      <c r="C55" s="30">
         <v>582</v>
       </c>
-      <c r="D55" s="39">
+      <c r="D55" s="30">
         <v>12</v>
       </c>
-      <c r="E55" s="38">
+      <c r="E55" s="27">
         <v>68</v>
       </c>
-      <c r="F55" s="9">
+      <c r="F55" s="29">
         <v>36</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G55" s="29">
         <v>32</v>
       </c>
-      <c r="H55" s="9">
+      <c r="H55" s="29">
         <v>4</v>
       </c>
-      <c r="I55" s="9">
-        <v>0</v>
-      </c>
-      <c r="J55" s="9">
+      <c r="I55" s="29">
+        <v>0</v>
+      </c>
+      <c r="J55" s="29">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K55" s="23"/>
+      <c r="L55" s="23"/>
+    </row>
+    <row r="56" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
         <v>43929</v>
       </c>
-      <c r="B56" s="32">
+      <c r="B56" s="30">
         <v>43</v>
       </c>
-      <c r="C56" s="32">
+      <c r="C56" s="30">
         <v>625</v>
       </c>
-      <c r="D56" s="39">
+      <c r="D56" s="30">
         <v>10</v>
       </c>
-      <c r="E56" s="38">
+      <c r="E56" s="27">
         <v>78</v>
       </c>
-      <c r="F56" s="9">
-        <v>43</v>
-      </c>
-      <c r="G56" s="9">
-        <v>39</v>
-      </c>
-      <c r="H56" s="9">
+      <c r="F56" s="27">
+        <v>45</v>
+      </c>
+      <c r="G56" s="29">
+        <v>41</v>
+      </c>
+      <c r="H56" s="29">
         <v>4</v>
       </c>
-      <c r="I56" s="9">
-        <v>0</v>
-      </c>
-      <c r="J56" s="9">
+      <c r="I56" s="29">
+        <v>0</v>
+      </c>
+      <c r="J56" s="29">
         <v>23</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K56" s="23"/>
+      <c r="L56" s="23"/>
+    </row>
+    <row r="57" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
         <v>43930</v>
       </c>
-      <c r="B57" s="39">
+      <c r="B57" s="30">
         <v>63</v>
       </c>
-      <c r="C57" s="39">
+      <c r="C57" s="30">
         <v>688</v>
       </c>
-      <c r="D57" s="39">
+      <c r="D57" s="30">
         <v>12</v>
       </c>
-      <c r="E57" s="38">
+      <c r="E57" s="27">
         <v>90</v>
       </c>
-      <c r="F57" s="9">
-        <v>43</v>
-      </c>
-      <c r="G57" s="9">
-        <v>39</v>
-      </c>
-      <c r="H57" s="9">
+      <c r="F57" s="27">
+        <v>50</v>
+      </c>
+      <c r="G57" s="29">
+        <v>46</v>
+      </c>
+      <c r="H57" s="29">
         <v>4</v>
       </c>
-      <c r="I57" s="9">
-        <v>0</v>
-      </c>
-      <c r="J57" s="9">
+      <c r="I57" s="29">
+        <v>0</v>
+      </c>
+      <c r="J57" s="29">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="17">
+      <c r="K57" s="23"/>
+      <c r="L57" s="23"/>
+    </row>
+    <row r="58" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="16">
         <v>43931</v>
       </c>
-      <c r="B58" s="39">
+      <c r="B58" s="30">
         <v>30</v>
       </c>
-      <c r="C58" s="39">
+      <c r="C58" s="30">
         <v>718</v>
       </c>
-      <c r="D58" s="39">
+      <c r="D58" s="30">
         <v>9</v>
       </c>
-      <c r="E58" s="38">
+      <c r="E58" s="27">
         <v>99</v>
       </c>
-      <c r="F58" s="9">
-        <v>43</v>
-      </c>
-      <c r="G58" s="9">
-        <v>39</v>
-      </c>
-      <c r="H58" s="9">
+      <c r="F58" s="29">
+        <v>51</v>
+      </c>
+      <c r="G58" s="29">
+        <v>47</v>
+      </c>
+      <c r="H58" s="29">
         <v>4</v>
       </c>
-      <c r="I58" s="9">
-        <v>0</v>
-      </c>
-      <c r="J58" s="9">
+      <c r="I58" s="29">
+        <v>0</v>
+      </c>
+      <c r="J58" s="29">
         <v>25</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K58" s="23"/>
+      <c r="L58" s="23"/>
+    </row>
+    <row r="59" spans="1:12" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="34">
         <v>43932</v>
       </c>
-      <c r="B59" s="39">
+      <c r="B59" s="35">
+        <v>25</v>
+      </c>
+      <c r="C59" s="35">
+        <v>743</v>
+      </c>
+      <c r="D59" s="35">
         <v>20</v>
       </c>
-      <c r="C59" s="39">
-        <v>738</v>
-      </c>
-      <c r="D59" s="39">
-        <v>14</v>
-      </c>
-      <c r="E59" s="38">
-        <v>113</v>
+      <c r="E59" s="19">
+        <v>119</v>
       </c>
       <c r="F59" s="9">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G59" s="9">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H59" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I59" s="9">
         <v>0</v>
       </c>
       <c r="J59" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="34"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A61" s="3"/>
-      <c r="B61" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="21"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="22"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="22"/>
-      <c r="I61" s="19"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B62" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62" s="23"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="22"/>
-      <c r="H62" s="22"/>
-      <c r="I62" s="19"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="D63" s="23"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="19"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="D64" s="36"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="44"/>
-      <c r="G64" s="33"/>
-      <c r="H64" s="44"/>
-      <c r="I64" s="33"/>
-      <c r="J64" s="33"/>
-    </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="C65" s="7"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="44"/>
-      <c r="I65" s="44"/>
-      <c r="J65" s="33"/>
-      <c r="K65" s="6"/>
-    </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="C66" s="7"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="37"/>
-      <c r="H66" s="44"/>
-      <c r="I66" s="44"/>
-      <c r="J66" s="33"/>
-      <c r="K66" s="6"/>
-    </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="C67" s="7"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="37"/>
-      <c r="H67" s="44"/>
-      <c r="I67" s="44"/>
-      <c r="J67" s="33"/>
-      <c r="K67" s="6"/>
-    </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="C68" s="7"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="41"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="37"/>
-      <c r="H68" s="37"/>
-      <c r="I68" s="37"/>
-      <c r="J68" s="37"/>
-      <c r="K68" s="6"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="34">
+        <v>43933</v>
+      </c>
+      <c r="B60" s="35">
+        <v>12</v>
+      </c>
+      <c r="C60" s="35">
+        <v>755</v>
+      </c>
+      <c r="D60" s="35">
+        <v>2</v>
+      </c>
+      <c r="E60" s="19">
+        <v>121</v>
+      </c>
+      <c r="F60" s="9">
+        <v>51</v>
+      </c>
+      <c r="G60" s="9">
+        <v>48</v>
+      </c>
+      <c r="H60" s="9">
+        <v>3</v>
+      </c>
+      <c r="I60" s="9">
+        <v>0</v>
+      </c>
+      <c r="J60" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="24"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="29"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A62" s="3"/>
+      <c r="B62" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="23"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="23"/>
+      <c r="J62" s="23"/>
+      <c r="K62" s="23"/>
+      <c r="L62" s="23"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B63" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="23"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="23"/>
+      <c r="L63" s="23"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="23"/>
+      <c r="L64" s="23"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="23"/>
+      <c r="L65" s="23"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="23"/>
+      <c r="L66" s="23"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="23"/>
+      <c r="H67" s="23"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="23"/>
+      <c r="K67" s="23"/>
+      <c r="L67" s="23"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="23"/>
+      <c r="K68" s="23"/>
+      <c r="L68" s="23"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="23"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="23"/>
+      <c r="L69" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2826,45 +2873,45 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="20.125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.125" style="11" customWidth="1"/>
+    <col min="5" max="6" width="20.125" style="10" customWidth="1"/>
     <col min="7" max="8" width="20.125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" x14ac:dyDescent="0.15">
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
@@ -2880,8 +2927,8 @@
       <c r="D2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="4">
         <v>0</v>
       </c>
@@ -2902,8 +2949,8 @@
       <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="4">
         <v>0</v>
       </c>
@@ -2924,8 +2971,8 @@
       <c r="D4" s="4">
         <v>3</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="4">
         <v>0</v>
       </c>
@@ -2946,8 +2993,8 @@
       <c r="D5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="4">
         <v>0</v>
       </c>
@@ -2968,8 +3015,8 @@
       <c r="D6" s="4">
         <v>3</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="4">
         <v>0</v>
       </c>
@@ -2990,8 +3037,8 @@
       <c r="D7" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="4">
         <v>0</v>
       </c>
@@ -3012,8 +3059,8 @@
       <c r="D8" s="4">
         <v>3</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="4">
         <v>0</v>
       </c>
@@ -3034,8 +3081,8 @@
       <c r="D9" s="4">
         <v>3</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="4">
         <v>0</v>
       </c>
@@ -3056,8 +3103,8 @@
       <c r="D10" s="4">
         <v>3</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="4">
         <v>0</v>
       </c>
@@ -3078,8 +3125,8 @@
       <c r="D11" s="4">
         <v>3</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
       <c r="G11" s="4">
         <v>0</v>
       </c>
@@ -3100,8 +3147,8 @@
       <c r="D12" s="4">
         <v>3</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="4">
         <v>0</v>
       </c>
@@ -3122,8 +3169,8 @@
       <c r="D13" s="4">
         <v>3</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="4">
         <v>0</v>
       </c>
@@ -3144,8 +3191,8 @@
       <c r="D14" s="4">
         <v>3</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="4">
         <v>0</v>
       </c>
@@ -3166,8 +3213,8 @@
       <c r="D15" s="4">
         <v>3</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="4">
         <v>0</v>
       </c>
@@ -3179,25 +3226,25 @@
       <c r="A16" s="3">
         <v>43914</v>
       </c>
-      <c r="B16" s="26">
-        <v>0</v>
-      </c>
-      <c r="C16" s="26">
-        <v>3</v>
-      </c>
-      <c r="D16" s="26">
-        <v>3</v>
-      </c>
-      <c r="E16" s="27">
-        <v>2</v>
-      </c>
-      <c r="F16" s="27">
-        <v>1</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
-      </c>
-      <c r="H16" s="26">
+      <c r="B16" s="18">
+        <v>0</v>
+      </c>
+      <c r="C16" s="18">
+        <v>3</v>
+      </c>
+      <c r="D16" s="18">
+        <v>3</v>
+      </c>
+      <c r="E16" s="19">
+        <v>2</v>
+      </c>
+      <c r="F16" s="19">
+        <v>1</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0</v>
+      </c>
+      <c r="H16" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3205,25 +3252,25 @@
       <c r="A17" s="3">
         <v>43915</v>
       </c>
-      <c r="B17" s="26">
-        <v>0</v>
-      </c>
-      <c r="C17" s="26">
-        <v>3</v>
-      </c>
-      <c r="D17" s="26">
-        <v>3</v>
-      </c>
-      <c r="E17" s="27">
-        <v>2</v>
-      </c>
-      <c r="F17" s="27">
-        <v>1</v>
-      </c>
-      <c r="G17" s="26">
-        <v>0</v>
-      </c>
-      <c r="H17" s="26">
+      <c r="B17" s="18">
+        <v>0</v>
+      </c>
+      <c r="C17" s="18">
+        <v>3</v>
+      </c>
+      <c r="D17" s="18">
+        <v>3</v>
+      </c>
+      <c r="E17" s="19">
+        <v>2</v>
+      </c>
+      <c r="F17" s="19">
+        <v>1</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0</v>
+      </c>
+      <c r="H17" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3231,25 +3278,25 @@
       <c r="A18" s="3">
         <v>43916</v>
       </c>
-      <c r="B18" s="26">
-        <v>0</v>
-      </c>
-      <c r="C18" s="26">
-        <v>3</v>
-      </c>
-      <c r="D18" s="26">
-        <v>2</v>
-      </c>
-      <c r="E18" s="26">
-        <v>1</v>
-      </c>
-      <c r="F18" s="26">
-        <v>1</v>
-      </c>
-      <c r="G18" s="26">
-        <v>0</v>
-      </c>
-      <c r="H18" s="26">
+      <c r="B18" s="18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="18">
         <v>1</v>
       </c>
     </row>
@@ -3257,25 +3304,25 @@
       <c r="A19" s="3">
         <v>43917</v>
       </c>
-      <c r="B19" s="26">
-        <v>0</v>
-      </c>
-      <c r="C19" s="26">
-        <v>3</v>
-      </c>
-      <c r="D19" s="26">
-        <v>2</v>
-      </c>
-      <c r="E19" s="26">
-        <v>1</v>
-      </c>
-      <c r="F19" s="26">
-        <v>1</v>
-      </c>
-      <c r="G19" s="26">
-        <v>0</v>
-      </c>
-      <c r="H19" s="26">
+      <c r="B19" s="18">
+        <v>0</v>
+      </c>
+      <c r="C19" s="18">
+        <v>3</v>
+      </c>
+      <c r="D19" s="18">
+        <v>2</v>
+      </c>
+      <c r="E19" s="18">
+        <v>1</v>
+      </c>
+      <c r="F19" s="18">
+        <v>1</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0</v>
+      </c>
+      <c r="H19" s="18">
         <v>1</v>
       </c>
     </row>
@@ -3283,25 +3330,25 @@
       <c r="A20" s="3">
         <v>43918</v>
       </c>
-      <c r="B20" s="26">
-        <v>0</v>
-      </c>
-      <c r="C20" s="26">
-        <v>3</v>
-      </c>
-      <c r="D20" s="26">
-        <v>2</v>
-      </c>
-      <c r="E20" s="26">
-        <v>1</v>
-      </c>
-      <c r="F20" s="26">
-        <v>1</v>
-      </c>
-      <c r="G20" s="26">
-        <v>0</v>
-      </c>
-      <c r="H20" s="26">
+      <c r="B20" s="18">
+        <v>0</v>
+      </c>
+      <c r="C20" s="18">
+        <v>3</v>
+      </c>
+      <c r="D20" s="18">
+        <v>2</v>
+      </c>
+      <c r="E20" s="18">
+        <v>1</v>
+      </c>
+      <c r="F20" s="18">
+        <v>1</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0</v>
+      </c>
+      <c r="H20" s="18">
         <v>1</v>
       </c>
     </row>
@@ -3309,25 +3356,25 @@
       <c r="A21" s="3">
         <v>43919</v>
       </c>
-      <c r="B21" s="26">
-        <v>0</v>
-      </c>
-      <c r="C21" s="26">
-        <v>3</v>
-      </c>
-      <c r="D21" s="26">
-        <v>2</v>
-      </c>
-      <c r="E21" s="26">
-        <v>1</v>
-      </c>
-      <c r="F21" s="26">
-        <v>1</v>
-      </c>
-      <c r="G21" s="26">
-        <v>0</v>
-      </c>
-      <c r="H21" s="26">
+      <c r="B21" s="18">
+        <v>0</v>
+      </c>
+      <c r="C21" s="18">
+        <v>3</v>
+      </c>
+      <c r="D21" s="18">
+        <v>2</v>
+      </c>
+      <c r="E21" s="18">
+        <v>1</v>
+      </c>
+      <c r="F21" s="18">
+        <v>1</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0</v>
+      </c>
+      <c r="H21" s="18">
         <v>1</v>
       </c>
     </row>
@@ -3347,13 +3394,13 @@
       <c r="E22" s="27">
         <v>2</v>
       </c>
-      <c r="F22" s="26">
-        <v>1</v>
-      </c>
-      <c r="G22" s="26">
-        <v>0</v>
-      </c>
-      <c r="H22" s="26">
+      <c r="F22" s="27">
+        <v>1</v>
+      </c>
+      <c r="G22" s="27">
+        <v>0</v>
+      </c>
+      <c r="H22" s="27">
         <v>1</v>
       </c>
     </row>
@@ -3373,13 +3420,13 @@
       <c r="E23" s="27">
         <v>4</v>
       </c>
-      <c r="F23" s="26">
-        <v>1</v>
-      </c>
-      <c r="G23" s="26">
-        <v>0</v>
-      </c>
-      <c r="H23" s="26">
+      <c r="F23" s="27">
+        <v>1</v>
+      </c>
+      <c r="G23" s="27">
+        <v>0</v>
+      </c>
+      <c r="H23" s="27">
         <v>1</v>
       </c>
     </row>
@@ -3399,13 +3446,13 @@
       <c r="E24" s="27">
         <v>4</v>
       </c>
-      <c r="F24" s="26">
-        <v>1</v>
-      </c>
-      <c r="G24" s="26">
-        <v>0</v>
-      </c>
-      <c r="H24" s="26">
+      <c r="F24" s="27">
+        <v>1</v>
+      </c>
+      <c r="G24" s="27">
+        <v>0</v>
+      </c>
+      <c r="H24" s="27">
         <v>1</v>
       </c>
     </row>
@@ -3425,13 +3472,13 @@
       <c r="E25" s="27">
         <v>4</v>
       </c>
-      <c r="F25" s="26">
-        <v>1</v>
-      </c>
-      <c r="G25" s="26">
-        <v>0</v>
-      </c>
-      <c r="H25" s="26">
+      <c r="F25" s="27">
+        <v>1</v>
+      </c>
+      <c r="G25" s="27">
+        <v>0</v>
+      </c>
+      <c r="H25" s="27">
         <v>1</v>
       </c>
     </row>
@@ -3451,13 +3498,13 @@
       <c r="E26" s="27">
         <v>4</v>
       </c>
-      <c r="F26" s="26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="26">
-        <v>0</v>
-      </c>
-      <c r="H26" s="26">
+      <c r="F26" s="27">
+        <v>1</v>
+      </c>
+      <c r="G26" s="27">
+        <v>0</v>
+      </c>
+      <c r="H26" s="27">
         <v>1</v>
       </c>
     </row>
@@ -3465,25 +3512,25 @@
       <c r="A27" s="3">
         <v>43925</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="29">
         <v>0</v>
       </c>
       <c r="C27" s="27">
         <v>6</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="29">
         <v>5</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="29">
         <v>4</v>
       </c>
-      <c r="F27" s="25">
-        <v>1</v>
-      </c>
-      <c r="G27" s="25">
-        <v>0</v>
-      </c>
-      <c r="H27" s="25">
+      <c r="F27" s="29">
+        <v>1</v>
+      </c>
+      <c r="G27" s="29">
+        <v>0</v>
+      </c>
+      <c r="H27" s="29">
         <v>1</v>
       </c>
     </row>
@@ -3503,13 +3550,13 @@
       <c r="E28" s="27">
         <v>4</v>
       </c>
-      <c r="F28" s="26">
-        <v>1</v>
-      </c>
-      <c r="G28" s="26">
-        <v>0</v>
-      </c>
-      <c r="H28" s="26">
+      <c r="F28" s="27">
+        <v>1</v>
+      </c>
+      <c r="G28" s="27">
+        <v>0</v>
+      </c>
+      <c r="H28" s="27">
         <v>1</v>
       </c>
     </row>
@@ -3529,13 +3576,13 @@
       <c r="E29" s="27">
         <v>4</v>
       </c>
-      <c r="F29" s="26">
-        <v>1</v>
-      </c>
-      <c r="G29" s="26">
-        <v>0</v>
-      </c>
-      <c r="H29" s="26">
+      <c r="F29" s="27">
+        <v>1</v>
+      </c>
+      <c r="G29" s="27">
+        <v>0</v>
+      </c>
+      <c r="H29" s="27">
         <v>1</v>
       </c>
     </row>
@@ -3555,13 +3602,13 @@
       <c r="E30" s="27">
         <v>4</v>
       </c>
-      <c r="F30" s="26">
-        <v>1</v>
-      </c>
-      <c r="G30" s="26">
-        <v>0</v>
-      </c>
-      <c r="H30" s="26">
+      <c r="F30" s="27">
+        <v>1</v>
+      </c>
+      <c r="G30" s="27">
+        <v>0</v>
+      </c>
+      <c r="H30" s="27">
         <v>1</v>
       </c>
     </row>
@@ -3581,18 +3628,18 @@
       <c r="E31" s="27">
         <v>6</v>
       </c>
-      <c r="F31" s="26">
-        <v>1</v>
-      </c>
-      <c r="G31" s="26">
-        <v>0</v>
-      </c>
-      <c r="H31" s="26">
+      <c r="F31" s="27">
+        <v>1</v>
+      </c>
+      <c r="G31" s="27">
+        <v>0</v>
+      </c>
+      <c r="H31" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="3">
+      <c r="A32" s="24">
         <v>43930</v>
       </c>
       <c r="B32" s="27">
@@ -3604,74 +3651,106 @@
       <c r="D32" s="27">
         <v>6</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="29">
         <v>5</v>
       </c>
-      <c r="F32" s="26">
-        <v>1</v>
-      </c>
-      <c r="G32" s="26">
-        <v>0</v>
-      </c>
-      <c r="H32" s="26">
+      <c r="F32" s="29">
+        <v>1</v>
+      </c>
+      <c r="G32" s="27">
+        <v>0</v>
+      </c>
+      <c r="H32" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A33" s="17">
+      <c r="A33" s="28">
         <v>43931</v>
       </c>
-      <c r="B33" s="38">
-        <v>0</v>
-      </c>
-      <c r="C33" s="38">
-        <v>8</v>
-      </c>
-      <c r="D33" s="38">
+      <c r="B33" s="27">
+        <v>1</v>
+      </c>
+      <c r="C33" s="27">
+        <v>9</v>
+      </c>
+      <c r="D33" s="27">
+        <v>7</v>
+      </c>
+      <c r="E33" s="29">
         <v>6</v>
       </c>
-      <c r="E33" s="38">
-        <v>5</v>
-      </c>
-      <c r="F33" s="35">
-        <v>1</v>
-      </c>
-      <c r="G33" s="35">
-        <v>0</v>
-      </c>
-      <c r="H33" s="35">
+      <c r="F33" s="29">
+        <v>1</v>
+      </c>
+      <c r="G33" s="27">
+        <v>0</v>
+      </c>
+      <c r="H33" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="34">
+      <c r="A34" s="28">
         <v>43932</v>
       </c>
-      <c r="B34" s="38">
-        <v>0</v>
-      </c>
-      <c r="C34" s="38">
-        <v>8</v>
-      </c>
-      <c r="D34" s="38">
+      <c r="B34" s="19">
+        <v>0</v>
+      </c>
+      <c r="C34" s="19">
+        <v>9</v>
+      </c>
+      <c r="D34" s="19">
+        <v>7</v>
+      </c>
+      <c r="E34" s="9">
         <v>6</v>
       </c>
-      <c r="E34" s="38">
-        <v>5</v>
-      </c>
-      <c r="F34" s="35">
-        <v>1</v>
-      </c>
-      <c r="G34" s="35">
-        <v>0</v>
-      </c>
-      <c r="H34" s="35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B36" s="1" t="s">
+      <c r="F34" s="9">
+        <v>1</v>
+      </c>
+      <c r="G34" s="19">
+        <v>0</v>
+      </c>
+      <c r="H34" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="24">
+        <v>43933</v>
+      </c>
+      <c r="B35" s="19">
+        <v>0</v>
+      </c>
+      <c r="C35" s="19">
+        <v>9</v>
+      </c>
+      <c r="D35" s="19">
         <v>7</v>
+      </c>
+      <c r="E35" s="9">
+        <v>6</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="19">
+        <v>0</v>
+      </c>
+      <c r="H35" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="28"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B37" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#158)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/kansensya_pcr_1.xlsx
+++ b/static/data/kansensya_pcr_1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\201058\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file.kobe.local\top\02_作業文書\01_組織\平成31年度\01_市長室\03_広報戦略部\01_広報課\04_HP\コロナ\HP作図\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">kobe!$A$1:$J$63</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">other!$A$1:$H$23</definedName>
   </definedNames>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -260,19 +260,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>※　38件調査中</t>
-    <rPh sb="4" eb="5">
-      <t>ケン</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>チョウサ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>チュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>入院・入居中</t>
     <rPh sb="0" eb="2">
       <t>ニュウイン</t>
@@ -286,6 +273,19 @@
     <t>入院・入居中</t>
     <rPh sb="3" eb="5">
       <t>ニュウキョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※　33件調査中</t>
+    <rPh sb="4" eb="5">
+      <t>ケン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>チョウサ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>チュウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -770,11 +770,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C16:C17"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -791,7 +791,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>9</v>
@@ -892,19 +892,19 @@
         <v>121</v>
       </c>
       <c r="C5" s="9">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D5" s="19">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E5" s="19">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F5" s="19">
         <v>4</v>
       </c>
       <c r="G5" s="19">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H5" s="19">
         <v>28</v>
@@ -948,13 +948,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
+      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -978,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
@@ -2590,11 +2590,11 @@
       <c r="E56" s="27">
         <v>78</v>
       </c>
-      <c r="F56" s="27">
-        <v>45</v>
-      </c>
-      <c r="G56" s="29">
-        <v>41</v>
+      <c r="F56" s="19">
+        <v>46</v>
+      </c>
+      <c r="G56" s="9">
+        <v>42</v>
       </c>
       <c r="H56" s="29">
         <v>4</v>
@@ -2624,11 +2624,11 @@
       <c r="E57" s="27">
         <v>90</v>
       </c>
-      <c r="F57" s="27">
-        <v>50</v>
-      </c>
-      <c r="G57" s="29">
-        <v>46</v>
+      <c r="F57" s="19">
+        <v>51</v>
+      </c>
+      <c r="G57" s="9">
+        <v>47</v>
       </c>
       <c r="H57" s="29">
         <v>4</v>
@@ -2658,11 +2658,11 @@
       <c r="E58" s="27">
         <v>99</v>
       </c>
-      <c r="F58" s="29">
-        <v>51</v>
-      </c>
-      <c r="G58" s="29">
-        <v>47</v>
+      <c r="F58" s="9">
+        <v>56</v>
+      </c>
+      <c r="G58" s="9">
+        <v>52</v>
       </c>
       <c r="H58" s="29">
         <v>4</v>
@@ -2693,10 +2693,10 @@
         <v>119</v>
       </c>
       <c r="F59" s="9">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G59" s="9">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H59" s="9">
         <v>3</v>
@@ -2713,10 +2713,10 @@
         <v>43933</v>
       </c>
       <c r="B60" s="35">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C60" s="35">
-        <v>755</v>
+        <v>790</v>
       </c>
       <c r="D60" s="35">
         <v>2</v>
@@ -2725,10 +2725,10 @@
         <v>121</v>
       </c>
       <c r="F60" s="9">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G60" s="9">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H60" s="9">
         <v>3</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B63" s="32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C63" s="23"/>
       <c r="D63" s="33"/>
@@ -2795,71 +2795,6 @@
       <c r="J64" s="23"/>
       <c r="K64" s="23"/>
       <c r="L64" s="23"/>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B65" s="23"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="23"/>
-      <c r="H65" s="23"/>
-      <c r="I65" s="23"/>
-      <c r="J65" s="23"/>
-      <c r="K65" s="23"/>
-      <c r="L65" s="23"/>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B66" s="23"/>
-      <c r="C66" s="23"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
-      <c r="H66" s="23"/>
-      <c r="I66" s="23"/>
-      <c r="J66" s="23"/>
-      <c r="K66" s="23"/>
-      <c r="L66" s="23"/>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B67" s="23"/>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B68" s="23"/>
-      <c r="C68" s="23"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="23"/>
-      <c r="H68" s="23"/>
-      <c r="I68" s="23"/>
-      <c r="J68" s="23"/>
-      <c r="K68" s="23"/>
-      <c r="L68" s="23"/>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B69" s="23"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="23"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="23"/>
-      <c r="G69" s="23"/>
-      <c r="H69" s="23"/>
-      <c r="I69" s="23"/>
-      <c r="J69" s="23"/>
-      <c r="K69" s="23"/>
-      <c r="L69" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2899,7 +2834,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>9</v>

</xml_diff>